<commit_message>
some files are modified correctly
</commit_message>
<xml_diff>
--- a/TestCases/08-PerformanceIndicatorHRM.xlsx
+++ b/TestCases/08-PerformanceIndicatorHRM.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
-    <sheet name="Performance Indicator HRM" sheetId="1" r:id="rId1"/>
+    <sheet name="TestScenario -Performance " sheetId="2" r:id="rId1"/>
+    <sheet name="TestCase -Performance Indicator" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="78">
   <si>
     <t>Project Name</t>
   </si>
@@ -98,9 +99,6 @@
     <t>TC_HRM_07</t>
   </si>
   <si>
-    <t>Integration Testing</t>
-  </si>
-  <si>
     <t>click on save button</t>
   </si>
   <si>
@@ -228,6 +226,39 @@
   </si>
   <si>
     <t>Mohamed Ovaize</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Smoke Testing</t>
+  </si>
+  <si>
+    <t>S No</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Check wheather login Url is working or not</t>
+  </si>
+  <si>
+    <t>Check wheather by leaving mandatory field blank is working or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check wheather adding Candidate detail window open by clicking Add button is working or not </t>
+  </si>
+  <si>
+    <t>Check wheather by adding valid performance Rating information is working or not</t>
+  </si>
+  <si>
+    <t>Check wheather by adding invalid performance Rating information is working or not</t>
+  </si>
+  <si>
+    <t>Check wheather by selecting checkbox and click delete button to the particular performanceIndicator is deleting or not</t>
+  </si>
+  <si>
+    <t>Check wheather adding existing information is working or not</t>
   </si>
 </sst>
 </file>
@@ -505,7 +536,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -582,12 +613,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -603,16 +628,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -788,6 +816,21 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1075,10 +1118,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:C28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="45.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="81" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="81" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="82"/>
+      <c r="C6" s="87"/>
+    </row>
+    <row r="7" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="83"/>
+      <c r="C7" s="88"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="29">
+        <v>1</v>
+      </c>
+      <c r="C8" s="94" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="95"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="96"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
+        <v>2</v>
+      </c>
+      <c r="C11" s="97" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="95"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="96"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="7">
+        <v>3</v>
+      </c>
+      <c r="C14" s="95" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="95"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="9"/>
+      <c r="C16" s="96"/>
+    </row>
+    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="7">
+        <v>4</v>
+      </c>
+      <c r="C17" s="95" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="95"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="96"/>
+    </row>
+    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
+        <v>5</v>
+      </c>
+      <c r="C20" s="97" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="95"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="95"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="7">
+        <v>6</v>
+      </c>
+      <c r="C23" s="97" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="95"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+      <c r="C25" s="96"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="7">
+        <v>7</v>
+      </c>
+      <c r="C26" s="97" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="95"/>
+    </row>
+    <row r="28" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="10"/>
+      <c r="C28" s="98"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+    <sheetView topLeftCell="A58" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1094,213 +1303,215 @@
   <sheetData>
     <row r="2" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="46" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="47"/>
-      <c r="G3" s="52" t="s">
+      <c r="F3" s="46"/>
+      <c r="G3" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="26"/>
+      <c r="I3" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="58"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="40"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="60"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="59"/>
     </row>
     <row r="5" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="43"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="62"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="52" t="s">
+      <c r="C6" s="37"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="46"/>
+      <c r="G6" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="28"/>
-      <c r="I6" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6" s="64"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="63"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="40"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="66"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="65"/>
     </row>
     <row r="8" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="43"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="68"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="67"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="70">
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="69">
         <v>43202</v>
       </c>
-      <c r="F9" s="71"/>
-      <c r="G9" s="52" t="s">
+      <c r="F9" s="70"/>
+      <c r="G9" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="76">
+      <c r="H9" s="26"/>
+      <c r="I9" s="75">
         <v>43203</v>
       </c>
-      <c r="J9" s="77"/>
+      <c r="J9" s="76"/>
     </row>
     <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="78"/>
-      <c r="J10" s="79"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="78"/>
     </row>
     <row r="11" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="81"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="80"/>
     </row>
     <row r="15" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="82" t="s">
+      <c r="B16" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="85" t="s">
+      <c r="C16" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="82" t="s">
+      <c r="D16" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="85" t="s">
+      <c r="E16" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="82" t="s">
+      <c r="F16" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="85" t="s">
+      <c r="G16" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="85" t="s">
+      <c r="H16" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="85" t="s">
+      <c r="I16" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="28" t="s">
+      <c r="J16" s="26" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="83"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="88"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="90"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="29"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="27"/>
     </row>
     <row r="18" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="84"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="89"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="30"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="28"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H19" s="36" t="s">
+      <c r="C19" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="I19" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="J19" s="36"/>
+      <c r="J19" s="33" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="23"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="8"/>
       <c r="H20" s="2"/>
       <c r="I20" s="5"/>
@@ -1311,7 +1522,7 @@
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="23"/>
+      <c r="F21" s="31"/>
       <c r="G21" s="8"/>
       <c r="H21" s="2"/>
       <c r="I21" s="5"/>
@@ -1320,15 +1531,15 @@
     <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="34"/>
-      <c r="F22" s="26" t="s">
-        <v>16</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="31"/>
       <c r="G22" s="8"/>
       <c r="H22" s="2"/>
       <c r="I22" s="5"/>
@@ -1338,8 +1549,8 @@
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="23"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="8"/>
       <c r="H23" s="2"/>
       <c r="I23" s="5"/>
@@ -1349,8 +1560,8 @@
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="23"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="8"/>
       <c r="H24" s="2"/>
       <c r="I24" s="5"/>
@@ -1359,22 +1570,20 @@
     <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="E25" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>16</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F25" s="31"/>
       <c r="G25" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="2"/>
@@ -1384,7 +1593,7 @@
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="24"/>
-      <c r="F26" s="23"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="8"/>
       <c r="H26" s="2"/>
       <c r="I26" s="5"/>
@@ -1395,7 +1604,7 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="25"/>
-      <c r="F27" s="27"/>
+      <c r="F27" s="35"/>
       <c r="G27" s="9"/>
       <c r="H27" s="3"/>
       <c r="I27" s="6"/>
@@ -1406,27 +1615,29 @@
         <v>18</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="13"/>
@@ -1455,25 +1666,29 @@
         <v>19</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F31" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J31" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
@@ -1501,14 +1716,12 @@
       <c r="B34" s="13"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E34" s="8">
         <v>10</v>
       </c>
-      <c r="F34" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="2"/>
       <c r="I34" s="5"/>
@@ -1540,14 +1753,12 @@
       <c r="B37" s="13"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E37" s="8">
         <v>20</v>
       </c>
-      <c r="F37" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="2"/>
       <c r="I37" s="5"/>
@@ -1579,14 +1790,12 @@
       <c r="B40" s="13"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E40" s="8">
         <v>100</v>
       </c>
-      <c r="F40" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="2"/>
       <c r="I40" s="5"/>
@@ -1618,12 +1827,12 @@
       <c r="B43" s="13"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="E43" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="2"/>
       <c r="I43" s="5"/>
@@ -1656,25 +1865,29 @@
         <v>20</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E46" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F46" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J46" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="13"/>
@@ -1702,14 +1915,12 @@
       <c r="B49" s="13"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E49" s="21">
         <v>2</v>
       </c>
-      <c r="F49" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="F49" s="8"/>
       <c r="G49" s="8"/>
       <c r="H49" s="2"/>
       <c r="I49" s="5"/>
@@ -1741,14 +1952,12 @@
       <c r="B52" s="13"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E52" s="8">
         <v>100</v>
       </c>
-      <c r="F52" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="F52" s="8"/>
       <c r="G52" s="8"/>
       <c r="H52" s="2"/>
       <c r="I52" s="5"/>
@@ -1780,14 +1989,12 @@
       <c r="B55" s="13"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E55" s="8">
         <v>80</v>
       </c>
-      <c r="F55" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="F55" s="8"/>
       <c r="G55" s="8"/>
       <c r="H55" s="2"/>
       <c r="I55" s="5"/>
@@ -1819,12 +2026,12 @@
       <c r="B58" s="13"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="E58" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F58" s="8"/>
       <c r="G58" s="8"/>
       <c r="H58" s="2"/>
       <c r="I58" s="5"/>
@@ -1857,25 +2064,29 @@
         <v>21</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E61" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F61" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J61" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="13"/>
@@ -1903,12 +2114,12 @@
       <c r="B64" s="13"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F64" s="8"/>
       <c r="G64" s="8"/>
       <c r="H64" s="2"/>
       <c r="I64" s="5"/>
@@ -1940,12 +2151,12 @@
       <c r="B67" s="13"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E67" s="8"/>
-      <c r="F67" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F67" s="8"/>
       <c r="G67" s="8"/>
       <c r="H67" s="2"/>
       <c r="I67" s="5"/>
@@ -1977,12 +2188,12 @@
       <c r="B70" s="13"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F70" s="8"/>
       <c r="G70" s="8"/>
       <c r="H70" s="2"/>
       <c r="I70" s="5"/>
@@ -2014,12 +2225,12 @@
       <c r="B73" s="13"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E73" s="8"/>
-      <c r="F73" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="E73" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F73" s="8"/>
       <c r="G73" s="8"/>
       <c r="H73" s="2"/>
       <c r="I73" s="5"/>
@@ -2052,26 +2263,28 @@
         <v>22</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E76" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F76" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G76" s="92" t="s">
-        <v>34</v>
+      <c r="G76" s="91" t="s">
+        <v>33</v>
       </c>
       <c r="H76" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I76" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="I76" s="18" t="s">
+      <c r="J76" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="J76" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
@@ -2080,7 +2293,7 @@
       <c r="D77" s="8"/>
       <c r="E77" s="8"/>
       <c r="F77" s="8"/>
-      <c r="G77" s="93"/>
+      <c r="G77" s="92"/>
       <c r="H77" s="16"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
@@ -2091,7 +2304,7 @@
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
       <c r="F78" s="8"/>
-      <c r="G78" s="93"/>
+      <c r="G78" s="92"/>
       <c r="H78" s="16"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
@@ -2100,15 +2313,13 @@
       <c r="B79" s="13"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E79" s="8">
         <v>10</v>
       </c>
-      <c r="F79" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G79" s="93"/>
+      <c r="F79" s="8"/>
+      <c r="G79" s="92"/>
       <c r="H79" s="16"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
@@ -2119,7 +2330,7 @@
       <c r="D80" s="8"/>
       <c r="E80" s="8"/>
       <c r="F80" s="8"/>
-      <c r="G80" s="93"/>
+      <c r="G80" s="92"/>
       <c r="H80" s="16"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
@@ -2130,7 +2341,7 @@
       <c r="D81" s="8"/>
       <c r="E81" s="8"/>
       <c r="F81" s="8"/>
-      <c r="G81" s="93"/>
+      <c r="G81" s="92"/>
       <c r="H81" s="16"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
@@ -2139,15 +2350,13 @@
       <c r="B82" s="13"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E82" s="8">
         <v>20</v>
       </c>
-      <c r="F82" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G82" s="93"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="92"/>
       <c r="H82" s="16"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
@@ -2158,7 +2367,7 @@
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
       <c r="F83" s="8"/>
-      <c r="G83" s="93"/>
+      <c r="G83" s="92"/>
       <c r="H83" s="16"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
@@ -2169,7 +2378,7 @@
       <c r="D84" s="8"/>
       <c r="E84" s="8"/>
       <c r="F84" s="8"/>
-      <c r="G84" s="93"/>
+      <c r="G84" s="92"/>
       <c r="H84" s="16"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
@@ -2178,15 +2387,13 @@
       <c r="B85" s="13"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E85" s="8">
         <v>100</v>
       </c>
-      <c r="F85" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G85" s="93"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="92"/>
       <c r="H85" s="16"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
@@ -2197,7 +2404,7 @@
       <c r="D86" s="8"/>
       <c r="E86" s="8"/>
       <c r="F86" s="8"/>
-      <c r="G86" s="93"/>
+      <c r="G86" s="92"/>
       <c r="H86" s="16"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
@@ -2208,7 +2415,7 @@
       <c r="D87" s="8"/>
       <c r="E87" s="8"/>
       <c r="F87" s="8"/>
-      <c r="G87" s="93"/>
+      <c r="G87" s="92"/>
       <c r="H87" s="16"/>
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
@@ -2217,13 +2424,13 @@
       <c r="B88" s="13"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E88" s="8"/>
-      <c r="F88" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G88" s="93"/>
+      <c r="E88" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F88" s="8"/>
+      <c r="G88" s="92"/>
       <c r="H88" s="16"/>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
@@ -2234,7 +2441,7 @@
       <c r="D89" s="8"/>
       <c r="E89" s="8"/>
       <c r="F89" s="8"/>
-      <c r="G89" s="93"/>
+      <c r="G89" s="92"/>
       <c r="H89" s="16"/>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
@@ -2245,7 +2452,7 @@
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
-      <c r="G90" s="94"/>
+      <c r="G90" s="93"/>
       <c r="H90" s="17"/>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
@@ -2255,25 +2462,29 @@
         <v>23</v>
       </c>
       <c r="C91" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D91" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D91" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E91" s="7"/>
+      <c r="E91" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="F91" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="J91" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="J91" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B92" s="13"/>
@@ -2298,19 +2509,13 @@
       <c r="J93" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="142">
+  <mergeCells count="124">
     <mergeCell ref="B76:B90"/>
     <mergeCell ref="C76:C90"/>
-    <mergeCell ref="F76:F78"/>
     <mergeCell ref="G76:G90"/>
     <mergeCell ref="B61:B75"/>
     <mergeCell ref="C61:C75"/>
-    <mergeCell ref="F61:F63"/>
     <mergeCell ref="G61:G75"/>
-    <mergeCell ref="F79:F81"/>
-    <mergeCell ref="F82:F84"/>
-    <mergeCell ref="F73:F75"/>
-    <mergeCell ref="F70:F72"/>
     <mergeCell ref="B3:D5"/>
     <mergeCell ref="E3:F5"/>
     <mergeCell ref="G3:H5"/>
@@ -2337,20 +2542,18 @@
     <mergeCell ref="C25:C27"/>
     <mergeCell ref="D25:D27"/>
     <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F25:F27"/>
     <mergeCell ref="G25:G27"/>
     <mergeCell ref="J16:J18"/>
     <mergeCell ref="C19:C21"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F22:F24"/>
     <mergeCell ref="G19:G24"/>
     <mergeCell ref="H19:H24"/>
     <mergeCell ref="H25:H27"/>
+    <mergeCell ref="F19:F27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="D28:D30"/>
@@ -2360,19 +2563,6 @@
     <mergeCell ref="H28:H30"/>
     <mergeCell ref="I28:I30"/>
     <mergeCell ref="J28:J30"/>
-    <mergeCell ref="J31:J45"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="F43:F45"/>
     <mergeCell ref="B31:B45"/>
     <mergeCell ref="C31:C45"/>
     <mergeCell ref="G31:G45"/>
@@ -2384,15 +2574,19 @@
     <mergeCell ref="B46:B60"/>
     <mergeCell ref="E55:E57"/>
     <mergeCell ref="D55:D57"/>
-    <mergeCell ref="F52:F54"/>
     <mergeCell ref="E52:E54"/>
     <mergeCell ref="D52:D54"/>
-    <mergeCell ref="F55:F57"/>
-    <mergeCell ref="F49:F51"/>
     <mergeCell ref="E49:E51"/>
     <mergeCell ref="D49:D51"/>
     <mergeCell ref="D46:D48"/>
     <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F31:F45"/>
+    <mergeCell ref="F46:F60"/>
+    <mergeCell ref="F61:F75"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="E37:E39"/>
     <mergeCell ref="H76:H90"/>
     <mergeCell ref="I76:I90"/>
     <mergeCell ref="J76:J90"/>
@@ -2400,14 +2594,13 @@
     <mergeCell ref="E82:E84"/>
     <mergeCell ref="D85:D87"/>
     <mergeCell ref="E85:E87"/>
-    <mergeCell ref="F85:F87"/>
     <mergeCell ref="E88:E90"/>
     <mergeCell ref="D79:D81"/>
     <mergeCell ref="E79:E81"/>
     <mergeCell ref="D88:D90"/>
-    <mergeCell ref="F88:F90"/>
     <mergeCell ref="D76:D78"/>
     <mergeCell ref="E76:E78"/>
+    <mergeCell ref="F76:F90"/>
     <mergeCell ref="G91:G93"/>
     <mergeCell ref="H91:H93"/>
     <mergeCell ref="I91:I93"/>
@@ -2421,26 +2614,26 @@
     <mergeCell ref="I46:I60"/>
     <mergeCell ref="H46:H60"/>
     <mergeCell ref="G46:G60"/>
-    <mergeCell ref="F46:F48"/>
     <mergeCell ref="D31:D33"/>
     <mergeCell ref="E31:E33"/>
-    <mergeCell ref="F31:F33"/>
     <mergeCell ref="H61:H75"/>
     <mergeCell ref="I61:I75"/>
     <mergeCell ref="J61:J75"/>
     <mergeCell ref="D64:D66"/>
     <mergeCell ref="E64:E66"/>
-    <mergeCell ref="F64:F66"/>
     <mergeCell ref="D67:D69"/>
     <mergeCell ref="E67:E69"/>
-    <mergeCell ref="F67:F69"/>
     <mergeCell ref="D70:D72"/>
     <mergeCell ref="E70:E72"/>
     <mergeCell ref="D73:D75"/>
     <mergeCell ref="E73:E75"/>
-    <mergeCell ref="F58:F60"/>
     <mergeCell ref="E58:E60"/>
     <mergeCell ref="D58:D60"/>
+    <mergeCell ref="J31:J45"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="E43:E45"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E28" r:id="rId1"/>

</xml_diff>